<commit_message>
add custom table  organism_pub fixed minor bug
</commit_message>
<xml_diff>
--- a/TEST_FILES/TEST_MCL_DATA.xlsx
+++ b/TEST_FILES/TEST_MCL_DATA.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CC258E0E-89DF-4D86-BCC6-5871E8DD64F5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="2" r:id="rId1"/>
@@ -15,32 +16,35 @@
     <sheet name="dataset" sheetId="4" r:id="rId6"/>
     <sheet name="db" sheetId="12" r:id="rId7"/>
     <sheet name="descriptor_fb" sheetId="10" r:id="rId8"/>
-    <sheet name="genotype_snp_marker_column" sheetId="21" r:id="rId9"/>
-    <sheet name="image" sheetId="23" r:id="rId10"/>
-    <sheet name="library" sheetId="18" r:id="rId11"/>
-    <sheet name="map_position" sheetId="20" r:id="rId12"/>
-    <sheet name="map" sheetId="19" r:id="rId13"/>
-    <sheet name="marker" sheetId="14" r:id="rId14"/>
-    <sheet name="MTL" sheetId="15" r:id="rId15"/>
-    <sheet name="organism" sheetId="11" r:id="rId16"/>
-    <sheet name="phenotype2" sheetId="5" r:id="rId17"/>
-    <sheet name="Progeny" sheetId="8" r:id="rId18"/>
-    <sheet name="QTL" sheetId="16" r:id="rId19"/>
-    <sheet name="site" sheetId="6" r:id="rId20"/>
-    <sheet name="stock" sheetId="7" r:id="rId21"/>
-    <sheet name="trait" sheetId="17" r:id="rId22"/>
-    <sheet name="genotype" sheetId="24" r:id="rId23"/>
-    <sheet name="genotype_b" sheetId="25" r:id="rId24"/>
+    <sheet name="descriptor" sheetId="29" r:id="rId9"/>
+    <sheet name="genotype_snp_marker_column" sheetId="21" r:id="rId10"/>
+    <sheet name="image" sheetId="23" r:id="rId11"/>
+    <sheet name="organism" sheetId="11" r:id="rId12"/>
+    <sheet name="library" sheetId="18" r:id="rId13"/>
+    <sheet name="map_position" sheetId="20" r:id="rId14"/>
+    <sheet name="qtl_trait_data" sheetId="28" r:id="rId15"/>
+    <sheet name="map" sheetId="19" r:id="rId16"/>
+    <sheet name="marker" sheetId="14" r:id="rId17"/>
+    <sheet name="MTL" sheetId="15" r:id="rId18"/>
+    <sheet name="phenotype" sheetId="5" r:id="rId19"/>
+    <sheet name="Progeny" sheetId="8" r:id="rId20"/>
+    <sheet name="QTL" sheetId="16" r:id="rId21"/>
+    <sheet name="site" sheetId="6" r:id="rId22"/>
+    <sheet name="stock" sheetId="7" r:id="rId23"/>
+    <sheet name="trait" sheetId="17" r:id="rId24"/>
+    <sheet name="genotype" sheetId="24" r:id="rId25"/>
+    <sheet name="genotype_b" sheetId="25" r:id="rId26"/>
+    <sheet name="genotype_c" sheetId="27" r:id="rId27"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">Progeny!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">Progeny!#REF!</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="559">
   <si>
     <t>*contact_name</t>
   </si>
@@ -840,9 +844,6 @@
     <t>mcl_test_genotype</t>
   </si>
   <si>
-    <t>mcl_test_file_name</t>
-  </si>
-  <si>
     <t>mcl_test_image_name</t>
   </si>
   <si>
@@ -1317,24 +1318,15 @@
     <t>*name</t>
   </si>
   <si>
-    <t>mcl_prop_contact</t>
-  </si>
-  <si>
     <t>mcl_prop_contact_definition</t>
   </si>
   <si>
-    <t>##mcl_prop_contact</t>
-  </si>
-  <si>
     <t>mcl_contactprop</t>
   </si>
   <si>
     <t>mcl_prop_marker_definition</t>
   </si>
   <si>
-    <t>mcl_prop_marker</t>
-  </si>
-  <si>
     <t>mcl_prop_contact_alias</t>
   </si>
   <si>
@@ -1344,16 +1336,397 @@
     <t>mcl_markerprop</t>
   </si>
   <si>
-    <t>##mcl_prop_marker</t>
-  </si>
-  <si>
     <t>mcl_test_cv</t>
+  </si>
+  <si>
+    <t>mcl_test_prop_contact</t>
+  </si>
+  <si>
+    <t>mcl_test_prop_marker</t>
+  </si>
+  <si>
+    <t>##mcl_test_prop_contact</t>
+  </si>
+  <si>
+    <t>##mcl_test_prop_marker</t>
+  </si>
+  <si>
+    <t>mcl_test_qtl_label_01</t>
+  </si>
+  <si>
+    <t>mcl_test_qtl_label_02</t>
+  </si>
+  <si>
+    <t>mcl_test_locus_3a</t>
+  </si>
+  <si>
+    <t>mcl_test_locus_4a;mcl_test_marker_4</t>
+  </si>
+  <si>
+    <t>mcl_test_locus_4b</t>
+  </si>
+  <si>
+    <t>mcl_test_locus_4a;mcl_test_locus_4b</t>
+  </si>
+  <si>
+    <t>mcl_test_mtl_name_01</t>
+  </si>
+  <si>
+    <t>mcl_test_GRIN_ID_001;mcl_test_GRIN_ID_002</t>
+  </si>
+  <si>
+    <t>mcl_test_mtl_name_02</t>
+  </si>
+  <si>
+    <t>October 60</t>
+  </si>
+  <si>
+    <t>3-79</t>
+  </si>
+  <si>
+    <t>1/2/2018</t>
+  </si>
+  <si>
+    <t>0034</t>
+  </si>
+  <si>
+    <t>$mcl_test_marker_5</t>
+  </si>
+  <si>
+    <t>$mcl_test_marker_6</t>
+  </si>
+  <si>
+    <t>101 | 100</t>
+  </si>
+  <si>
+    <t>90 | 101</t>
+  </si>
+  <si>
+    <t>100 | 100</t>
+  </si>
+  <si>
+    <t>clone_id</t>
+  </si>
+  <si>
+    <t>mcl_test_clone_id_ssr_B01</t>
+  </si>
+  <si>
+    <t>mcl_test_clone_id_ssr_B02</t>
+  </si>
+  <si>
+    <t>mcl_test_clone_id_ssr_C0</t>
+  </si>
+  <si>
+    <t>mcl_test_clone_id_ssr_C1</t>
+  </si>
+  <si>
+    <t>80 |89</t>
+  </si>
+  <si>
+    <t>AAAT[A|T]TTAU[C/A/T]CCCGCG</t>
+  </si>
+  <si>
+    <t>AAATA]A|T[TTAU</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>geographic_origin</t>
+  </si>
+  <si>
+    <t>haploid_chromosome_number</t>
+  </si>
+  <si>
+    <t>genome_size</t>
+  </si>
+  <si>
+    <t>ploidy</t>
+  </si>
+  <si>
+    <t>growth_habit</t>
+  </si>
+  <si>
+    <t>propagation_method</t>
+  </si>
+  <si>
+    <t>usage</t>
+  </si>
+  <si>
+    <t>hybrid_parentage</t>
+  </si>
+  <si>
+    <t>resistance_to_biotic_stress</t>
+  </si>
+  <si>
+    <t>resistance_to_abiotic_stress</t>
+  </si>
+  <si>
+    <t>alias_scientific</t>
+  </si>
+  <si>
+    <t>alias_synonym</t>
+  </si>
+  <si>
+    <t>alias_common</t>
+  </si>
+  <si>
+    <t>fertile_with</t>
+  </si>
+  <si>
+    <t>sterile_with</t>
+  </si>
+  <si>
+    <t>incompatible_with</t>
+  </si>
+  <si>
+    <t>GRIN Taxonomy ID</t>
+  </si>
+  <si>
+    <t>g1</t>
+  </si>
+  <si>
+    <t>g2</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>stock photo</t>
+  </si>
+  <si>
+    <t>organism</t>
+  </si>
+  <si>
+    <t>organism photo</t>
+  </si>
+  <si>
+    <t>mcl_test_image_comments</t>
+  </si>
+  <si>
+    <t>mcl_test_s_image_comments</t>
+  </si>
+  <si>
+    <t>trait photo</t>
+  </si>
+  <si>
+    <t>trait</t>
+  </si>
+  <si>
+    <t>mcl_test_organism.png</t>
+  </si>
+  <si>
+    <t>mcl_test_stock.png</t>
+  </si>
+  <si>
+    <t>mcl_test_trait.png</t>
+  </si>
+  <si>
+    <t>mcl_test_file_name.jpg</t>
+  </si>
+  <si>
+    <t>mcl_test_t_image_comments</t>
+  </si>
+  <si>
+    <t>mcl_test_o1_image_comments</t>
+  </si>
+  <si>
+    <t>mcl_test_o2_image_comments</t>
+  </si>
+  <si>
+    <t>mcl_test_o3_image_comments</t>
+  </si>
+  <si>
+    <t>mcl_test_o4_image_comments</t>
+  </si>
+  <si>
+    <t>organism_fertile</t>
+  </si>
+  <si>
+    <t>mcl_test_organism_fertile.png</t>
+  </si>
+  <si>
+    <t>organism fertile photo</t>
+  </si>
+  <si>
+    <t>mcl_test_organism_sterile.png</t>
+  </si>
+  <si>
+    <t>organism_sterile</t>
+  </si>
+  <si>
+    <t>organism sterile photo</t>
+  </si>
+  <si>
+    <t>organism incompatible photo</t>
+  </si>
+  <si>
+    <t>organism_incompatible</t>
+  </si>
+  <si>
+    <t>mcl_test_organism_incompatible.png</t>
+  </si>
+  <si>
+    <t>mcl_test_genus_fertile</t>
+  </si>
+  <si>
+    <t>mcl_test_genus_sterile</t>
+  </si>
+  <si>
+    <t>mcl_test_species_sterile</t>
+  </si>
+  <si>
+    <t>mcl_test_species_fertile</t>
+  </si>
+  <si>
+    <t>mcl_test_genus_fertile_ic</t>
+  </si>
+  <si>
+    <t>mcl_test_species_ic</t>
+  </si>
+  <si>
+    <t>g3</t>
+  </si>
+  <si>
+    <t>g4</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>7227;7228;7229</t>
+  </si>
+  <si>
+    <t>AAATTTAU[-/T]CCCGCG</t>
+  </si>
+  <si>
+    <t>mcl_test_marker_7</t>
+  </si>
+  <si>
+    <t>mcl_test_locus_3b</t>
+  </si>
+  <si>
+    <t>mcl_test_locus_3s</t>
+  </si>
+  <si>
+    <t>test-data</t>
+  </si>
+  <si>
+    <t>* dataset_name</t>
+  </si>
+  <si>
+    <t>* stock_name</t>
+  </si>
+  <si>
+    <t>* genus</t>
+  </si>
+  <si>
+    <t>* species</t>
+  </si>
+  <si>
+    <t>* descriptor</t>
+  </si>
+  <si>
+    <t>* mean</t>
+  </si>
+  <si>
+    <t>min_value</t>
+  </si>
+  <si>
+    <t>max_value</t>
+  </si>
+  <si>
+    <t>standard_deviation</t>
+  </si>
+  <si>
+    <t>coefficient_of_variation</t>
+  </si>
+  <si>
+    <t>skewness</t>
+  </si>
+  <si>
+    <t>h2</t>
+  </si>
+  <si>
+    <t>CI_90</t>
+  </si>
+  <si>
+    <t>mcl_test_dataset_qtl_data</t>
+  </si>
+  <si>
+    <t>phenotype</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>mcl_test_qtl_descriptor_a</t>
+  </si>
+  <si>
+    <t>mcl_test_qtl_descriptor_b</t>
+  </si>
+  <si>
+    <t>mcl_test_qtl_descriptor_c</t>
+  </si>
+  <si>
+    <t>descriptor_name</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>QTL descriptor</t>
+  </si>
+  <si>
+    <t>mcl_test_qtl_descriptor_a1</t>
+  </si>
+  <si>
+    <t>mcl_test_qtl_descriptor_bata</t>
+  </si>
+  <si>
+    <t>row1</t>
+  </si>
+  <si>
+    <t>row2</t>
+  </si>
+  <si>
+    <t>row3</t>
+  </si>
+  <si>
+    <t>row4</t>
+  </si>
+  <si>
+    <t>row5</t>
+  </si>
+  <si>
+    <t>row6</t>
+  </si>
+  <si>
+    <t>row7</t>
+  </si>
+  <si>
+    <t>row8</t>
+  </si>
+  <si>
+    <t>row9</t>
+  </si>
+  <si>
+    <t>row10</t>
+  </si>
+  <si>
+    <t>row11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1481,13 +1854,13 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1536,6 +1909,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1552,7 +1931,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1626,9 +2005,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1637,12 +2013,29 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1982,11 +2375,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,63 +2406,63 @@
     <col min="20" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:19" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="G1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="62" t="s">
+      <c r="H1" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="62" t="s">
+      <c r="I1" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="62" t="s">
+      <c r="K1" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="62" t="s">
+      <c r="L1" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="62" t="s">
+      <c r="M1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="62" t="s">
+      <c r="N1" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="62" t="s">
+      <c r="O1" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="62" t="s">
+      <c r="P1" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="62" t="s">
+      <c r="Q1" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="62" t="s">
+      <c r="R1" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="62" t="s">
-        <v>427</v>
+      <c r="S1" s="59" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -2128,7 +2521,7 @@
         <v>222</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -2139,47 +2532,54 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>162</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>266</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>405</v>
       </c>
       <c r="B2" t="s">
-        <v>267</v>
+        <v>226</v>
       </c>
       <c r="C2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D2" t="s">
-        <v>221</v>
+        <v>264</v>
+      </c>
+      <c r="E2" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2188,7 +2588,431 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>490</v>
+      </c>
+      <c r="B3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C3" t="s">
+        <v>482</v>
+      </c>
+      <c r="D3" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>491</v>
+      </c>
+      <c r="B4" t="s">
+        <v>488</v>
+      </c>
+      <c r="C4" t="s">
+        <v>487</v>
+      </c>
+      <c r="D4" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>489</v>
+      </c>
+      <c r="B5" t="s">
+        <v>483</v>
+      </c>
+      <c r="C5" t="s">
+        <v>484</v>
+      </c>
+      <c r="D5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>499</v>
+      </c>
+      <c r="B6" t="s">
+        <v>498</v>
+      </c>
+      <c r="C6" t="s">
+        <v>500</v>
+      </c>
+      <c r="D6" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>501</v>
+      </c>
+      <c r="B7" t="s">
+        <v>502</v>
+      </c>
+      <c r="C7" t="s">
+        <v>503</v>
+      </c>
+      <c r="D7" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>506</v>
+      </c>
+      <c r="B8" t="s">
+        <v>505</v>
+      </c>
+      <c r="C8" t="s">
+        <v>504</v>
+      </c>
+      <c r="D8" t="s">
+        <v>497</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:X12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>463</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>464</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>465</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>466</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>467</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>468</v>
+      </c>
+      <c r="L1" s="37" t="s">
+        <v>469</v>
+      </c>
+      <c r="M1" s="37" t="s">
+        <v>470</v>
+      </c>
+      <c r="N1" s="37" t="s">
+        <v>471</v>
+      </c>
+      <c r="O1" s="37" t="s">
+        <v>472</v>
+      </c>
+      <c r="P1" s="37" t="s">
+        <v>473</v>
+      </c>
+      <c r="Q1" s="37" t="s">
+        <v>474</v>
+      </c>
+      <c r="R1" s="37" t="s">
+        <v>475</v>
+      </c>
+      <c r="S1" s="37" t="s">
+        <v>476</v>
+      </c>
+      <c r="T1" s="37" t="s">
+        <v>477</v>
+      </c>
+      <c r="U1" s="37" t="s">
+        <v>478</v>
+      </c>
+      <c r="V1" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="W1" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" s="37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D2" t="s">
+        <v>515</v>
+      </c>
+      <c r="E2" t="s">
+        <v>479</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" t="s">
+        <v>515</v>
+      </c>
+      <c r="E3" t="s">
+        <v>479</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D4" t="s">
+        <v>515</v>
+      </c>
+      <c r="E4" t="s">
+        <v>479</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5" t="s">
+        <v>332</v>
+      </c>
+      <c r="D5" t="s">
+        <v>516</v>
+      </c>
+      <c r="E5" t="s">
+        <v>479</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>507</v>
+      </c>
+      <c r="B6" t="s">
+        <v>510</v>
+      </c>
+      <c r="D6" t="s">
+        <v>516</v>
+      </c>
+      <c r="E6" t="s">
+        <v>480</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>508</v>
+      </c>
+      <c r="B7" t="s">
+        <v>509</v>
+      </c>
+      <c r="D7" t="s">
+        <v>516</v>
+      </c>
+      <c r="E7" t="s">
+        <v>513</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>511</v>
+      </c>
+      <c r="B8" t="s">
+        <v>512</v>
+      </c>
+      <c r="D8" t="s">
+        <v>516</v>
+      </c>
+      <c r="E8" t="s">
+        <v>514</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="70" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="69" t="s">
+        <v>263</v>
+      </c>
+      <c r="B12" s="69" t="s">
+        <v>264</v>
+      </c>
+      <c r="D12" s="69" t="s">
+        <v>515</v>
+      </c>
+      <c r="E12" s="69" t="s">
+        <v>479</v>
+      </c>
+      <c r="F12" s="69">
+        <v>1</v>
+      </c>
+      <c r="G12" s="69">
+        <v>4</v>
+      </c>
+      <c r="R12" s="69">
+        <v>2765</v>
+      </c>
+      <c r="S12" s="69">
+        <v>2766</v>
+      </c>
+      <c r="T12" s="69">
+        <v>2767</v>
+      </c>
+      <c r="V12" s="69" t="s">
+        <v>517</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2223,7 +3047,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B2" t="s">
         <v>167</v>
@@ -2243,12 +3067,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2260,7 +3084,7 @@
     <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -2311,40 +3135,31 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B2" t="s">
         <v>270</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>271</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>272</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>273</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>274</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>275</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>276</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>277</v>
-      </c>
-      <c r="I2" t="s">
-        <v>278</v>
-      </c>
-      <c r="J2" t="s">
-        <v>279</v>
-      </c>
-      <c r="K2" t="s">
-        <v>280</v>
-      </c>
-      <c r="L2" t="s">
-        <v>281</v>
       </c>
       <c r="M2" t="s">
         <v>221</v>
@@ -2352,19 +3167,19 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" t="s">
         <v>282</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" t="s">
+        <v>272</v>
+      </c>
+      <c r="I3" t="s">
         <v>283</v>
-      </c>
-      <c r="C3" t="s">
-        <v>272</v>
-      </c>
-      <c r="D3" t="s">
-        <v>273</v>
-      </c>
-      <c r="I3" t="s">
-        <v>284</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -2372,34 +3187,431 @@
       <c r="K3">
         <v>8</v>
       </c>
-      <c r="L3">
-        <v>9</v>
-      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B4" t="s">
         <v>285</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" t="s">
+        <v>272</v>
+      </c>
+      <c r="I4" t="s">
         <v>286</v>
       </c>
-      <c r="C4" t="s">
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B5" t="s">
+        <v>437</v>
+      </c>
+      <c r="C5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D5" t="s">
         <v>272</v>
       </c>
-      <c r="D4" t="s">
-        <v>273</v>
-      </c>
-      <c r="I4" t="s">
-        <v>287</v>
-      </c>
-      <c r="J4">
+      <c r="J5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>320</v>
+      </c>
+      <c r="B6" t="s">
+        <v>520</v>
+      </c>
+      <c r="C6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" t="s">
+        <v>272</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>320</v>
+      </c>
+      <c r="B7" t="s">
+        <v>521</v>
+      </c>
+      <c r="C7" t="s">
+        <v>271</v>
+      </c>
+      <c r="D7" t="s">
+        <v>272</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>436</v>
+      </c>
+      <c r="C8" t="s">
+        <v>271</v>
+      </c>
+      <c r="D8" t="s">
+        <v>272</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>436</v>
+      </c>
+      <c r="C9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D9" t="s">
+        <v>272</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>436</v>
+      </c>
+      <c r="C10" t="s">
+        <v>271</v>
+      </c>
+      <c r="D10" t="s">
+        <v>272</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>436</v>
+      </c>
+      <c r="C11" t="s">
+        <v>271</v>
+      </c>
+      <c r="D11" t="s">
+        <v>272</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="K11">
+        <v>9</v>
+      </c>
+      <c r="L11">
         <v>8</v>
       </c>
-      <c r="K4">
+    </row>
+    <row r="14" spans="1:13" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="70" t="s">
+        <v>522</v>
+      </c>
+      <c r="I14" s="69" t="s">
+        <v>548</v>
+      </c>
+      <c r="J14" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="K14" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="L14" s="37" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="69" t="s">
+        <v>269</v>
+      </c>
+      <c r="I15" s="69" t="s">
+        <v>549</v>
+      </c>
+      <c r="J15" s="69" t="s">
+        <v>278</v>
+      </c>
+      <c r="K15" s="69" t="s">
+        <v>279</v>
+      </c>
+      <c r="L15" s="69" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="69" t="s">
+        <v>281</v>
+      </c>
+      <c r="I16" s="69" t="s">
+        <v>550</v>
+      </c>
+      <c r="J16" s="69">
         <v>0</v>
       </c>
-      <c r="L4">
+      <c r="K16" s="69">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="69" t="s">
+        <v>284</v>
+      </c>
+      <c r="I17" s="69" t="s">
+        <v>551</v>
+      </c>
+      <c r="J17" s="69">
+        <v>5.67</v>
+      </c>
+      <c r="K17" s="69">
         <v>0</v>
+      </c>
+      <c r="L17" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="69" t="s">
+        <v>320</v>
+      </c>
+      <c r="I18" s="69" t="s">
+        <v>552</v>
+      </c>
+      <c r="L18" s="69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="69" t="s">
+        <v>320</v>
+      </c>
+      <c r="I19" s="69" t="s">
+        <v>553</v>
+      </c>
+      <c r="K19" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="69" t="s">
+        <v>320</v>
+      </c>
+      <c r="I20" s="69" t="s">
+        <v>554</v>
+      </c>
+      <c r="J20" s="69">
+        <v>0</v>
+      </c>
+      <c r="K20" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="69" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="69" t="s">
+        <v>436</v>
+      </c>
+      <c r="I21" s="69" t="s">
+        <v>555</v>
+      </c>
+      <c r="J21" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="69" t="s">
+        <v>436</v>
+      </c>
+      <c r="I22" s="69" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="69" t="s">
+        <v>436</v>
+      </c>
+      <c r="I23" s="69" t="s">
+        <v>557</v>
+      </c>
+      <c r="J23" s="69">
+        <v>0</v>
+      </c>
+      <c r="K23" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="69" t="s">
+        <v>436</v>
+      </c>
+      <c r="I24" s="69" t="s">
+        <v>558</v>
+      </c>
+      <c r="J24" s="69">
+        <v>3</v>
+      </c>
+      <c r="K24" s="69">
+        <v>9</v>
+      </c>
+      <c r="L24" s="69">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>548</v>
+      </c>
+      <c r="J25" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="K25" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="L25" s="37" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>400</v>
+      </c>
+      <c r="I26" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>400</v>
+      </c>
+      <c r="I27" t="s">
+        <v>550</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>400</v>
+      </c>
+      <c r="I28" t="s">
+        <v>551</v>
+      </c>
+      <c r="J28">
+        <v>4</v>
+      </c>
+      <c r="K28">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>400</v>
+      </c>
+      <c r="I29" t="s">
+        <v>552</v>
+      </c>
+      <c r="J29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>400</v>
+      </c>
+      <c r="I30" t="s">
+        <v>553</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>400</v>
+      </c>
+      <c r="I31" t="s">
+        <v>554</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>168</v>
+      </c>
+      <c r="I32" t="s">
+        <v>555</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>168</v>
+      </c>
+      <c r="I33" t="s">
+        <v>556</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>168</v>
+      </c>
+      <c r="I34" t="s">
+        <v>557</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>168</v>
+      </c>
+      <c r="I35" t="s">
+        <v>558</v>
+      </c>
+      <c r="J35">
+        <v>3</v>
+      </c>
+      <c r="K35">
+        <v>9</v>
+      </c>
+      <c r="L35">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2407,8 +3619,244 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3632BB1D-2306-4381-A85E-4D179BD65415}">
+  <dimension ref="A1:Q6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
+        <v>523</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>524</v>
+      </c>
+      <c r="C1" s="71" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="71" t="s">
+        <v>525</v>
+      </c>
+      <c r="E1" s="71" t="s">
+        <v>526</v>
+      </c>
+      <c r="F1" s="71" t="s">
+        <v>527</v>
+      </c>
+      <c r="G1" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="71" t="s">
+        <v>528</v>
+      </c>
+      <c r="I1" s="71" t="s">
+        <v>529</v>
+      </c>
+      <c r="J1" s="71" t="s">
+        <v>530</v>
+      </c>
+      <c r="K1" s="71" t="s">
+        <v>531</v>
+      </c>
+      <c r="L1" s="71" t="s">
+        <v>532</v>
+      </c>
+      <c r="M1" s="71" t="s">
+        <v>533</v>
+      </c>
+      <c r="N1" s="71" t="s">
+        <v>534</v>
+      </c>
+      <c r="O1" s="71" t="s">
+        <v>535</v>
+      </c>
+      <c r="P1" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="71" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="G2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2">
+        <v>1.5</v>
+      </c>
+      <c r="I2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J2">
+        <v>7.8</v>
+      </c>
+      <c r="K2">
+        <v>2.7</v>
+      </c>
+      <c r="L2">
+        <v>5.6</v>
+      </c>
+      <c r="M2">
+        <v>7.8</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+      <c r="P2" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E3" t="s">
+        <v>264</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="G3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H3">
+        <v>1.3</v>
+      </c>
+      <c r="I3">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E4" t="s">
+        <v>264</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="G4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H4">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" t="s">
+        <v>263</v>
+      </c>
+      <c r="E5" t="s">
+        <v>264</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="G5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5">
+        <v>2.5</v>
+      </c>
+      <c r="I5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D6" t="s">
+        <v>263</v>
+      </c>
+      <c r="E6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="G6" t="s">
+        <v>168</v>
+      </c>
+      <c r="H6">
+        <v>3.4</v>
+      </c>
+      <c r="I6">
+        <v>3.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2482,7 +3930,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B2" t="s">
         <v>263</v>
@@ -2494,31 +3942,31 @@
         <v>233</v>
       </c>
       <c r="E2" t="s">
+        <v>287</v>
+      </c>
+      <c r="F2" t="s">
         <v>288</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>289</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>290</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>291</v>
-      </c>
-      <c r="I2" t="s">
-        <v>292</v>
       </c>
       <c r="J2" t="s">
         <v>226</v>
       </c>
       <c r="K2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L2" t="s">
         <v>221</v>
       </c>
       <c r="M2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N2" t="s">
         <v>206</v>
@@ -2532,12 +3980,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AK12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AA26" sqref="AA26"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2689,13 +4137,13 @@
       <c r="AJ1" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" s="63" t="s">
+      <c r="AK1" s="60" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B2" t="s">
         <v>181</v>
@@ -2710,79 +4158,79 @@
         <v>207</v>
       </c>
       <c r="F2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I2" t="s">
         <v>174</v>
       </c>
       <c r="J2" t="s">
+        <v>295</v>
+      </c>
+      <c r="K2" t="s">
         <v>296</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>297</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>298</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>299</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>300</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q2" t="s">
         <v>301</v>
       </c>
-      <c r="P2" t="s">
-        <v>269</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>302</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>303</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>304</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>305</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>306</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>307</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>308</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>309</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>310</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>311</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>312</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>313</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>314</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>315</v>
       </c>
       <c r="AF2" t="s">
         <v>221</v>
       </c>
       <c r="AG2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AI2" t="s">
         <v>206</v>
@@ -2791,12 +4239,12 @@
         <v>1</v>
       </c>
       <c r="AK2" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B3" t="s">
         <v>181</v>
@@ -2808,10 +4256,10 @@
         <v>264</v>
       </c>
       <c r="E3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I3" t="s">
         <v>175</v>
@@ -2819,7 +4267,7 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
         <v>181</v>
@@ -2831,10 +4279,10 @@
         <v>264</v>
       </c>
       <c r="E4" t="s">
+        <v>318</v>
+      </c>
+      <c r="F4" t="s">
         <v>319</v>
-      </c>
-      <c r="F4" t="s">
-        <v>320</v>
       </c>
       <c r="L4" t="s">
         <v>179</v>
@@ -2848,7 +4296,7 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B5" t="s">
         <v>181</v>
@@ -2860,7 +4308,10 @@
         <v>264</v>
       </c>
       <c r="E5" t="s">
-        <v>397</v>
+        <v>396</v>
+      </c>
+      <c r="F5" t="s">
+        <v>437</v>
       </c>
       <c r="I5" t="s">
         <v>177</v>
@@ -2868,7 +4319,7 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B6" t="s">
         <v>181</v>
@@ -2880,7 +4331,10 @@
         <v>264</v>
       </c>
       <c r="E6" t="s">
-        <v>397</v>
+        <v>396</v>
+      </c>
+      <c r="F6" t="s">
+        <v>440</v>
       </c>
       <c r="I6" t="s">
         <v>176</v>
@@ -2888,19 +4342,19 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B7" t="s">
         <v>182</v>
       </c>
       <c r="C7" t="s">
+        <v>323</v>
+      </c>
+      <c r="D7" t="s">
         <v>324</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>325</v>
-      </c>
-      <c r="E7" t="s">
-        <v>326</v>
       </c>
       <c r="I7" t="s">
         <v>183</v>
@@ -2908,27 +4362,55 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B8" t="s">
         <v>182</v>
       </c>
       <c r="C8" t="s">
+        <v>323</v>
+      </c>
+      <c r="D8" t="s">
         <v>324</v>
       </c>
-      <c r="D8" t="s">
-        <v>325</v>
-      </c>
       <c r="E8" t="s">
-        <v>413</v>
+        <v>412</v>
+      </c>
+      <c r="I8" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>519</v>
+      </c>
+      <c r="B9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" t="s">
+        <v>263</v>
+      </c>
+      <c r="D9" t="s">
+        <v>264</v>
+      </c>
+      <c r="I9" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
+        <v>326</v>
+      </c>
+      <c r="H12" t="s">
         <v>327</v>
       </c>
-      <c r="H12" t="s">
-        <v>328</v>
+      <c r="I12" t="s">
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -2937,17 +4419,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="43" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" style="43" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="43" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="43" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" style="43" bestFit="1" customWidth="1"/>
@@ -3014,7 +4496,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B2" s="43" t="s">
         <v>263</v>
@@ -3023,34 +4505,71 @@
         <v>264</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F2" s="43" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G2" s="43" t="s">
         <v>207</v>
       </c>
       <c r="H2" s="43" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I2" s="43" t="s">
         <v>239</v>
       </c>
       <c r="J2" s="43" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K2" s="43" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L2" s="43" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M2" s="43" t="s">
         <v>206</v>
       </c>
       <c r="O2" s="43">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>441</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>263</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>264</v>
+      </c>
+      <c r="K3" t="s">
+        <v>438</v>
+      </c>
+      <c r="L3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>443</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>263</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>264</v>
+      </c>
+      <c r="K4" t="s">
+        <v>439</v>
+      </c>
+      <c r="L4" t="s">
+        <v>438</v>
+      </c>
+      <c r="O4" s="43">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3058,73 +4577,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>324</v>
-      </c>
-      <c r="B3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>332</v>
-      </c>
-      <c r="B4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>263</v>
-      </c>
-      <c r="B5" t="s">
-        <v>333</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomLeft" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3224,25 +4684,25 @@
         <v>16</v>
       </c>
       <c r="V1" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="W1" s="14" t="s">
         <v>338</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="X1" s="14" t="s">
         <v>339</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="Y1" s="20" t="s">
         <v>340</v>
       </c>
-      <c r="Y1" s="20" t="s">
+      <c r="Z1" s="22" t="s">
         <v>341</v>
       </c>
-      <c r="Z1" s="22" t="s">
+      <c r="AA1" s="22" t="s">
         <v>342</v>
       </c>
-      <c r="AA1" s="22" t="s">
-        <v>343</v>
-      </c>
       <c r="AB1" s="48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3259,10 +4719,10 @@
         <v>264</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>344</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>345</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>206</v>
@@ -3271,40 +4731,40 @@
         <v>224</v>
       </c>
       <c r="I2" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="J2" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="K2" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>356</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>357</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>221</v>
@@ -3316,10 +4776,10 @@
         <v>56.987000000000002</v>
       </c>
       <c r="X2" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="Y2" s="45" t="s">
         <v>393</v>
-      </c>
-      <c r="Y2" s="45" t="s">
-        <v>394</v>
       </c>
       <c r="Z2" s="3">
         <v>45</v>
@@ -3328,7 +4788,7 @@
         <v>42.4</v>
       </c>
       <c r="AB2" s="49" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="3" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3345,10 +4805,10 @@
         <v>264</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>206</v>
@@ -3357,40 +4817,40 @@
         <v>224</v>
       </c>
       <c r="I3" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="J3" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>356</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>357</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>221</v>
@@ -3402,7 +4862,7 @@
         <v>204</v>
       </c>
       <c r="Y3" s="45" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="Z3" s="3">
         <v>57.4</v>
@@ -3437,7 +4897,7 @@
         <v>50.6</v>
       </c>
       <c r="AB8" s="49" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -3468,7 +4928,7 @@
         <v>197</v>
       </c>
       <c r="X11" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Y11" s="5" t="s">
         <v>199</v>
@@ -3505,8 +4965,110 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15" style="2" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="2"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" style="4" customWidth="1"/>
+    <col min="14" max="15" width="8.85546875" style="8"/>
+    <col min="16" max="16" width="34.5703125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" style="8"/>
+    <col min="19" max="19" width="17.85546875" style="4" customWidth="1"/>
+    <col min="20" max="22" width="8.85546875" style="8"/>
+    <col min="23" max="16384" width="8.85546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="6"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="7"/>
+      <c r="S1" s="8"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3575,7 +5137,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>207</v>
@@ -3596,13 +5158,13 @@
         <v>239</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -3611,18 +5173,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA2"/>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
@@ -3738,10 +5300,10 @@
         <v>240</v>
       </c>
       <c r="B2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D2" t="s">
         <v>263</v>
@@ -3750,7 +5312,7 @@
         <v>264</v>
       </c>
       <c r="F2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>224</v>
@@ -3759,58 +5321,104 @@
         <v>207</v>
       </c>
       <c r="J2" t="s">
+        <v>359</v>
+      </c>
+      <c r="K2" t="s">
         <v>360</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>361</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>362</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>363</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>364</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>365</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>366</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>367</v>
       </c>
-      <c r="R2" t="s">
-        <v>368</v>
-      </c>
       <c r="S2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="T2" t="s">
         <v>221</v>
       </c>
       <c r="U2" t="s">
+        <v>368</v>
+      </c>
+      <c r="V2" t="s">
         <v>369</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>370</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>371</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>372</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>373</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>374</v>
       </c>
       <c r="AA2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" t="s">
+        <v>435</v>
+      </c>
+      <c r="D3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E3" t="s">
+        <v>264</v>
+      </c>
+      <c r="F3" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>438</v>
+      </c>
+      <c r="R3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4" t="s">
+        <v>436</v>
+      </c>
+      <c r="D4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E4" t="s">
+        <v>264</v>
+      </c>
+      <c r="F4" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>439</v>
+      </c>
+      <c r="R4" t="s">
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -3818,114 +5426,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="2"/>
-    <col min="12" max="12" width="17.85546875" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" style="4" customWidth="1"/>
-    <col min="14" max="15" width="8.85546875" style="8"/>
-    <col min="16" max="16" width="34.5703125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" style="4" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" style="8"/>
-    <col min="19" max="19" width="17.85546875" style="4" customWidth="1"/>
-    <col min="20" max="22" width="8.85546875" style="8"/>
-    <col min="23" max="16384" width="8.85546875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="7"/>
-      <c r="S1" s="8"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4004,10 +5510,10 @@
         <v>217</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>375</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>376</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>212</v>
@@ -4028,18 +5534,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U10"/>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A9"/>
+      <selection activeCell="A7" sqref="A7:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="124.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="17" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
@@ -4143,22 +5649,22 @@
         <v>264</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>377</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>378</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>239</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>381</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>226</v>
@@ -4167,19 +5673,19 @@
         <v>226</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>385</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>221</v>
@@ -4190,10 +5696,10 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>66</v>
@@ -4207,7 +5713,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>66</v>
@@ -4221,7 +5727,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>66</v>
@@ -4235,10 +5741,10 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>66</v>
@@ -4252,7 +5758,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>66</v>
@@ -4263,10 +5769,13 @@
       <c r="E7" t="s">
         <v>264</v>
       </c>
+      <c r="F7" s="2" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>66</v>
@@ -4280,7 +5789,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>66</v>
@@ -4293,31 +5802,100 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>390</v>
+      <c r="A10" s="39" t="s">
+        <v>444</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>66</v>
       </c>
       <c r="D10" t="s">
+        <v>263</v>
+      </c>
+      <c r="E10" t="s">
+        <v>264</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>446</v>
+      </c>
+      <c r="K10" s="39" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
+        <v>445</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>263</v>
+      </c>
+      <c r="E11" t="s">
+        <v>264</v>
+      </c>
+      <c r="K11" s="39" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
+        <v>446</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>263</v>
+      </c>
+      <c r="E12" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="s">
+        <v>447</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" t="s">
+        <v>263</v>
+      </c>
+      <c r="E13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>323</v>
+      </c>
+      <c r="E16" t="s">
         <v>324</v>
       </c>
-      <c r="E10" t="s">
-        <v>325</v>
+      <c r="J16" s="39" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4344,13 +5922,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B2" s="41" t="s">
         <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D2" t="s">
         <v>231</v>
@@ -4364,7 +5942,7 @@
         <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D3" t="s">
         <v>231</v>
@@ -4378,7 +5956,7 @@
         <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D4" t="s">
         <v>231</v>
@@ -4392,7 +5970,7 @@
         <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D5" t="s">
         <v>231</v>
@@ -4406,7 +5984,7 @@
         <v>170</v>
       </c>
       <c r="C6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D6" t="s">
         <v>231</v>
@@ -4418,12 +5996,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4445,48 +6023,48 @@
         <v>32</v>
       </c>
       <c r="C1" s="51" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1" s="51" t="s">
         <v>399</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>400</v>
       </c>
       <c r="E1" s="52" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="52" t="s">
+        <v>400</v>
+      </c>
+      <c r="G1" s="51" t="s">
         <v>401</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="H1" s="51" t="s">
         <v>402</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="I1" s="51" t="s">
         <v>403</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="J1" s="51" t="s">
         <v>404</v>
-      </c>
-      <c r="J1" s="51" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="C2" s="59" t="s">
-        <v>416</v>
+        <v>387</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>415</v>
       </c>
       <c r="D2" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="E2" s="60" t="s">
-        <v>417</v>
+      <c r="E2" s="57" t="s">
+        <v>416</v>
       </c>
       <c r="F2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G2" s="53">
         <v>143</v>
@@ -4500,22 +6078,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>420</v>
+        <v>388</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>419</v>
       </c>
       <c r="D3" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="E3" s="60" t="s">
-        <v>418</v>
+      <c r="E3" s="57" t="s">
+        <v>417</v>
       </c>
       <c r="F3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G3" s="53">
         <v>143</v>
@@ -4529,22 +6107,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="C4" s="59" t="s">
-        <v>421</v>
+        <v>389</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>420</v>
       </c>
       <c r="D4" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="E4" s="60" t="s">
-        <v>419</v>
+      <c r="E4" s="57" t="s">
+        <v>418</v>
       </c>
       <c r="F4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G4" s="53">
         <v>143</v>
@@ -4562,108 +6140,109 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="21.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="64" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1" s="64" t="s">
         <v>399</v>
       </c>
-      <c r="D1" s="56" t="s">
-        <v>400</v>
-      </c>
-      <c r="E1" s="57" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="58" t="s">
-        <v>411</v>
-      </c>
-      <c r="G1" s="58" t="s">
+      <c r="E1" s="52" t="s">
+        <v>453</v>
+      </c>
+      <c r="F1" s="63" t="s">
         <v>410</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="G1" s="63" t="s">
+        <v>409</v>
+      </c>
+      <c r="H1" s="63" t="s">
+        <v>413</v>
+      </c>
+      <c r="I1" s="63" t="s">
         <v>414</v>
       </c>
-      <c r="I1" s="58" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="65" t="s">
+        <v>407</v>
+      </c>
+      <c r="B2" s="66" t="s">
+        <v>387</v>
+      </c>
+      <c r="C2" s="56" t="s">
         <v>415</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="C2" s="59" t="s">
-        <v>416</v>
       </c>
       <c r="D2" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="E2" t="s">
-        <v>417</v>
-      </c>
-      <c r="F2" s="58">
+      <c r="E2" s="66" t="s">
+        <v>454</v>
+      </c>
+      <c r="F2" s="55">
         <v>107</v>
       </c>
-      <c r="G2" s="58">
+      <c r="G2" s="55">
         <v>107</v>
       </c>
-      <c r="H2" s="58">
+      <c r="H2" s="55">
         <v>172</v>
       </c>
-      <c r="I2" s="58">
+      <c r="I2" s="55">
         <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>420</v>
+      <c r="A3" s="65" t="s">
+        <v>407</v>
+      </c>
+      <c r="B3" s="66" t="s">
+        <v>388</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>419</v>
       </c>
       <c r="D3" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="E3" t="s">
-        <v>418</v>
-      </c>
-      <c r="F3" s="58">
+      <c r="E3" s="66" t="s">
+        <v>455</v>
+      </c>
+      <c r="F3" s="55">
         <v>107</v>
       </c>
-      <c r="G3" s="58">
+      <c r="G3" s="55">
         <v>107</v>
       </c>
-      <c r="H3" s="58">
+      <c r="H3" s="55">
         <v>164</v>
       </c>
-      <c r="I3" s="58">
+      <c r="I3" s="55">
         <v>176</v>
       </c>
     </row>
@@ -4672,12 +6251,106 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{763B009D-4724-479E-B9DD-7C5E4EC6E9C2}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="32"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>399</v>
+      </c>
+      <c r="E1" s="61" t="s">
+        <v>453</v>
+      </c>
+      <c r="F1" s="62" t="s">
+        <v>448</v>
+      </c>
+      <c r="G1" s="62" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="65" t="s">
+        <v>407</v>
+      </c>
+      <c r="B2" s="66" t="s">
+        <v>387</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2" s="66" t="s">
+        <v>456</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>450</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="65" t="s">
+        <v>407</v>
+      </c>
+      <c r="B3" s="66" t="s">
+        <v>388</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>419</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>457</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>452</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>458</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4691,14 +6364,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="58" t="s">
+        <v>422</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>421</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>423</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>422</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>424</v>
       </c>
       <c r="D1" s="28" t="s">
         <v>1</v>
@@ -4712,16 +6385,16 @@
         <v>232</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4729,16 +6402,16 @@
         <v>232</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -4748,7 +6421,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4779,7 +6452,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B3" t="s">
         <v>189</v>
@@ -4792,7 +6465,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4866,17 +6539,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="26" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -4980,7 +6653,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>159</v>
@@ -5023,7 +6696,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>159</v>
@@ -5040,7 +6713,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>159</v>
@@ -5057,7 +6730,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>159</v>
@@ -5070,6 +6743,23 @@
       </c>
       <c r="J8" s="2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
@@ -5083,7 +6773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5132,11 +6822,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5192,7 +6882,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>242</v>
@@ -5223,7 +6913,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>245</v>
@@ -5256,7 +6946,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>248</v>
@@ -5282,7 +6972,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>251</v>
@@ -5306,7 +6996,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>254</v>
@@ -5332,7 +7022,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>256</v>
@@ -5358,7 +7048,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>258</v>
@@ -5376,15 +7066,12 @@
         <v>231</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="16"/>
-    </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E11" s="46"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>260</v>
@@ -5414,57 +7101,116 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A05A0D-3D3F-44BE-B0D2-DCFD321D200B}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="B2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C2" t="s">
-        <v>263</v>
-      </c>
-      <c r="D2" t="s">
-        <v>264</v>
+    <row r="1" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>542</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>543</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="C2" s="72" t="s">
+        <v>546</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>185</v>
       </c>
       <c r="E2" t="s">
-        <v>265</v>
+        <v>244</v>
+      </c>
+      <c r="F2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>540</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>547</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F3" s="73" t="s">
+        <v>187</v>
+      </c>
+      <c r="G3" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>541</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="E4" t="s">
+        <v>250</v>
+      </c>
+      <c r="F4" s="73" t="s">
+        <v>544</v>
+      </c>
+      <c r="G4" t="s">
+        <v>545</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed some template. typo
</commit_message>
<xml_diff>
--- a/TEST_FILES/TEST_MCL_DATA.xlsx
+++ b/TEST_FILES/TEST_MCL_DATA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CC258E0E-89DF-4D86-BCC6-5871E8DD64F5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{96E73F92-9802-4F05-B577-FA05B031E8EC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="560">
   <si>
     <t>*contact_name</t>
   </si>
@@ -1721,6 +1721,9 @@
   </si>
   <si>
     <t>row11</t>
+  </si>
+  <si>
+    <t>0;1</t>
   </si>
 </sst>
 </file>
@@ -2724,8 +2727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2848,6 +2851,9 @@
       <c r="G2">
         <v>4</v>
       </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2868,6 +2874,9 @@
       <c r="G3">
         <v>4</v>
       </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2888,6 +2897,9 @@
       <c r="G4">
         <v>5</v>
       </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2907,6 +2919,9 @@
       </c>
       <c r="G5">
         <v>7</v>
+      </c>
+      <c r="W5" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -3071,7 +3086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+    <sheetView topLeftCell="D4" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>

</xml_diff>